<commit_message>
done DZ2 for economics
</commit_message>
<xml_diff>
--- a/Экономика часть 2/ДЗ2/Лист Microsoft Excel.xlsx
+++ b/Экономика часть 2/ДЗ2/Лист Microsoft Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Учёба\8 Семестр\Экономика часть 2\ДЗ2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41452B7-B258-4211-A03E-641C262C9E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCBD798-04E5-45FF-9DED-67112DDE4C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="221">
   <si>
     <t xml:space="preserve">Наименование показателя </t>
   </si>
@@ -1030,6 +1030,9 @@
   </si>
   <si>
     <t>Р-ПРОЧ%</t>
+  </si>
+  <si>
+    <t>CFO =</t>
   </si>
 </sst>
 </file>
@@ -1301,25 +1304,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1334,37 +1322,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1372,12 +1330,6 @@
     </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1408,6 +1360,57 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2190,6 +2193,526 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$D$144:$E$144</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #\ ##0_-;\-* #\ ##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>839</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C86B-48B8-99C3-1E8465882375}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1382672096"/>
+        <c:axId val="1382667520"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1382672096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1382667520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1382667520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-* #\ ##0_-;\-* #\ ##0_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1382672096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$D$110:$E$110</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #\ ##0_-;\-* #\ ##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>168071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>186299</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-79F8-4D28-B777-C8CF047C24F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$D$127:$E$127</c:f>
+              <c:numCache>
+                <c:formatCode>\(_-* #\ ##0_-\);\-* #\ ##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-167469</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-244062</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-79F8-4D28-B777-C8CF047C24F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$D$143:$E$143</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #\ ##0_-;\-* #\ ##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58602</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-79F8-4D28-B777-C8CF047C24F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1000039408"/>
+        <c:axId val="1000036496"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1000039408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1000036496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1000036496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-* #\ ##0_-;\-* #\ ##0_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1000039408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2310,6 +2833,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
@@ -3821,6 +4424,1012 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3958,6 +5567,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>366712</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1704975</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Диаграмма 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C440266-ADF4-46CF-81C7-93BEA723B1B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Диаграмма 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E59D446C-78FB-480C-BC7D-4C7F8312D601}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4231,8 +5912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:S189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K198" sqref="K198"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J118" sqref="J118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5335,15 +7016,15 @@
       <c r="J76" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="K76" s="32">
+      <c r="K76" s="28">
         <f>K47-K54-K55</f>
         <v>783970</v>
       </c>
-      <c r="L76" s="32">
+      <c r="L76" s="28">
         <f>L47-L54-L55</f>
         <v>736552</v>
       </c>
-      <c r="M76" s="32">
+      <c r="M76" s="28">
         <f>M47-M54-M55</f>
         <v>605021</v>
       </c>
@@ -5370,15 +7051,15 @@
       <c r="J77" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="K77" s="32">
+      <c r="K77" s="28">
         <f>K49-K55</f>
         <v>89966</v>
       </c>
-      <c r="L77" s="32">
+      <c r="L77" s="28">
         <f t="shared" ref="L77:M77" si="1">L49-L55</f>
         <v>206780</v>
       </c>
-      <c r="M77" s="32">
+      <c r="M77" s="28">
         <f t="shared" si="1"/>
         <v>100760</v>
       </c>
@@ -5399,24 +7080,24 @@
       </c>
     </row>
     <row r="78" spans="8:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H78" s="27" t="s">
+      <c r="H78" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="I78" s="29" t="s">
+      <c r="I78" s="61" t="s">
         <v>88</v>
       </c>
       <c r="J78" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="K78" s="33">
+      <c r="K78" s="63">
         <f>D7+D14</f>
         <v>689248</v>
       </c>
-      <c r="L78" s="33">
+      <c r="L78" s="63">
         <f t="shared" ref="L78:M78" si="2">E7+E14</f>
         <v>521696</v>
       </c>
-      <c r="M78" s="33">
+      <c r="M78" s="63">
         <f t="shared" si="2"/>
         <v>503327</v>
       </c>
@@ -5437,14 +7118,14 @@
       </c>
     </row>
     <row r="79" spans="8:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H79" s="28"/>
-      <c r="I79" s="30"/>
+      <c r="H79" s="60"/>
+      <c r="I79" s="62"/>
       <c r="J79" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="K79" s="28"/>
-      <c r="L79" s="28"/>
-      <c r="M79" s="28"/>
+      <c r="K79" s="60"/>
+      <c r="L79" s="60"/>
+      <c r="M79" s="60"/>
       <c r="P79" s="5" t="s">
         <v>77</v>
       </c>
@@ -5471,15 +7152,15 @@
       <c r="J80" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="K80" s="35">
+      <c r="K80" s="30">
         <f>K78/K47</f>
         <v>0.62487919420494831</v>
       </c>
-      <c r="L80" s="35">
+      <c r="L80" s="30">
         <f t="shared" ref="L80:M80" si="3">L78/L47</f>
         <v>0.50690452593326729</v>
       </c>
-      <c r="M80" s="35">
+      <c r="M80" s="30">
         <f t="shared" si="3"/>
         <v>0.55532422884353561</v>
       </c>
@@ -5494,15 +7175,15 @@
       <c r="J81" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="K81" s="32">
+      <c r="K81" s="28">
         <f>(K48+K49)/K53</f>
         <v>1.4069543477428983</v>
       </c>
-      <c r="L81" s="32">
+      <c r="L81" s="28">
         <f t="shared" ref="L81:M81" si="4">(L48+L49)/L53</f>
         <v>1.397294420488981</v>
       </c>
-      <c r="M81" s="32">
+      <c r="M81" s="28">
         <f t="shared" si="4"/>
         <v>1.4980736205850707</v>
       </c>
@@ -5538,21 +7219,21 @@
       <c r="J85" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="K85" s="35">
+      <c r="K85" s="30">
         <f>K53/K47</f>
         <v>0.71075511554745652</v>
       </c>
-      <c r="L85" s="35">
+      <c r="L85" s="30">
         <f t="shared" ref="L85:M85" si="5">L53/L47</f>
         <v>0.71566878485784802</v>
       </c>
-      <c r="M85" s="35">
+      <c r="M85" s="30">
         <f t="shared" si="5"/>
         <v>0.6675239362465053</v>
       </c>
     </row>
     <row r="86" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H86" s="34" t="s">
+      <c r="H86" s="29" t="s">
         <v>100</v>
       </c>
       <c r="I86" s="24" t="s">
@@ -5561,21 +7242,21 @@
       <c r="J86" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="K86" s="35">
+      <c r="K86" s="30">
         <f>(K54+K55)/K47</f>
         <v>0.28924488445254348</v>
       </c>
-      <c r="L86" s="35">
+      <c r="L86" s="30">
         <f t="shared" ref="L86:M86" si="6">(L54+L55)/L47</f>
         <v>0.28433121514215198</v>
       </c>
-      <c r="M86" s="35">
+      <c r="M86" s="30">
         <f t="shared" si="6"/>
         <v>0.3324760637534947</v>
       </c>
     </row>
-    <row r="87" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H87" s="34" t="s">
+    <row r="87" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H87" s="29" t="s">
         <v>103</v>
       </c>
       <c r="I87" s="24" t="s">
@@ -5584,15 +7265,15 @@
       <c r="J87" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K87" s="35">
+      <c r="K87" s="30">
         <f>K77/K53</f>
         <v>0.11475694222993227</v>
       </c>
-      <c r="L87" s="35">
+      <c r="L87" s="30">
         <f t="shared" ref="L87:M87" si="7">L77/L53</f>
         <v>0.28074053155785333</v>
       </c>
-      <c r="M87" s="35">
+      <c r="M87" s="30">
         <f t="shared" si="7"/>
         <v>0.16653967382950344</v>
       </c>
@@ -5607,15 +7288,15 @@
       <c r="J88" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="K88" s="35">
+      <c r="K88" s="30">
         <f>K77/K49</f>
         <v>0.21999481594146905</v>
       </c>
-      <c r="L88" s="35">
+      <c r="L88" s="30">
         <f t="shared" ref="L88:M88" si="8">L77/L49</f>
         <v>0.41440704800612455</v>
       </c>
-      <c r="M88" s="35">
+      <c r="M88" s="30">
         <f t="shared" si="8"/>
         <v>0.25110963243192053</v>
       </c>
@@ -5641,8 +7322,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H91" s="34" t="s">
+    <row r="91" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H91" s="29" t="s">
         <v>109</v>
       </c>
       <c r="I91" s="24" t="s">
@@ -5651,21 +7332,21 @@
       <c r="J91" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="K91" s="35">
+      <c r="K91" s="30">
         <f>D18/K55</f>
         <v>2.681672832152486E-2</v>
       </c>
-      <c r="L91" s="35">
+      <c r="L91" s="30">
         <f t="shared" ref="L91:M91" si="9">E18/L55</f>
         <v>2.7214423096667328E-2</v>
       </c>
-      <c r="M91" s="35">
+      <c r="M91" s="30">
         <f t="shared" si="9"/>
         <v>2.3670627855666742E-2</v>
       </c>
     </row>
-    <row r="92" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H92" s="31" t="s">
+    <row r="92" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H92" s="27" t="s">
         <v>112</v>
       </c>
       <c r="I92" s="24" t="s">
@@ -5674,15 +7355,15 @@
       <c r="J92" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="K92" s="35">
+      <c r="K92" s="30">
         <f>(D18+D16)/K55</f>
         <v>0.79315317574769573</v>
       </c>
-      <c r="L92" s="35">
+      <c r="L92" s="30">
         <f t="shared" ref="L92:M92" si="10">(E18+E16)/L55</f>
         <v>0.69745857261172217</v>
       </c>
-      <c r="M92" s="35">
+      <c r="M92" s="30">
         <f t="shared" si="10"/>
         <v>0.70727024049996834</v>
       </c>
@@ -5697,15 +7378,15 @@
       <c r="J93" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="K93" s="35">
+      <c r="K93" s="30">
         <f>K49/K55</f>
         <v>1.282042761301649</v>
       </c>
-      <c r="L93" s="35">
+      <c r="L93" s="30">
         <f t="shared" ref="L93:M93" si="11">L49/L55</f>
         <v>1.7076708259467894</v>
       </c>
-      <c r="M93" s="35">
+      <c r="M93" s="30">
         <f t="shared" si="11"/>
         <v>1.3353089361362267</v>
       </c>
@@ -5729,12 +7410,12 @@
       </c>
     </row>
     <row r="96" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="38" t="s">
+      <c r="B96" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="C96" s="39"/>
-      <c r="D96" s="39"/>
-      <c r="E96" s="39"/>
+      <c r="C96" s="56"/>
+      <c r="D96" s="56"/>
+      <c r="E96" s="56"/>
       <c r="F96" s="9"/>
     </row>
     <row r="97" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5744,23 +7425,23 @@
       <c r="C97" s="12">
         <v>4110</v>
       </c>
-      <c r="D97" s="46">
+      <c r="D97" s="33">
         <v>1450775</v>
       </c>
-      <c r="E97" s="46">
+      <c r="E97" s="33">
         <v>1272612</v>
       </c>
-      <c r="F97" s="46" t="s">
+      <c r="F97" s="33" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="98" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="40" t="s">
+      <c r="B98" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="C98" s="41"/>
-      <c r="D98" s="41"/>
-      <c r="E98" s="41"/>
+      <c r="C98" s="52"/>
+      <c r="D98" s="52"/>
+      <c r="E98" s="52"/>
       <c r="F98" s="9"/>
     </row>
     <row r="99" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5770,13 +7451,13 @@
       <c r="C99" s="4">
         <v>4111</v>
       </c>
-      <c r="D99" s="49">
+      <c r="D99" s="34">
         <v>1410093</v>
       </c>
-      <c r="E99" s="49">
+      <c r="E99" s="34">
         <v>1193013</v>
       </c>
-      <c r="F99" s="49" t="s">
+      <c r="F99" s="34" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5787,13 +7468,13 @@
       <c r="C100" s="4">
         <v>4112</v>
       </c>
-      <c r="D100" s="49">
+      <c r="D100" s="34">
         <v>26119</v>
       </c>
-      <c r="E100" s="49">
+      <c r="E100" s="34">
         <v>33529</v>
       </c>
-      <c r="F100" s="49" t="s">
+      <c r="F100" s="34" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5804,13 +7485,13 @@
       <c r="C101" s="4">
         <v>4113</v>
       </c>
-      <c r="D101" s="49" t="s">
+      <c r="D101" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E101" s="49" t="s">
+      <c r="E101" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F101" s="49" t="s">
+      <c r="F101" s="34" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5821,13 +7502,13 @@
       <c r="C102" s="4">
         <v>4119</v>
       </c>
-      <c r="D102" s="49">
+      <c r="D102" s="34">
         <v>14563</v>
       </c>
-      <c r="E102" s="49">
+      <c r="E102" s="34">
         <v>46071</v>
       </c>
-      <c r="F102" s="49" t="s">
+      <c r="F102" s="34" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5838,21 +7519,21 @@
       <c r="C103" s="4">
         <v>4120</v>
       </c>
-      <c r="D103" s="50">
+      <c r="D103" s="35">
         <v>1282704</v>
       </c>
-      <c r="E103" s="50">
+      <c r="E103" s="35">
         <v>1086313</v>
       </c>
-      <c r="F103" s="50"/>
+      <c r="F103" s="35"/>
     </row>
     <row r="104" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="40" t="s">
+      <c r="B104" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="C104" s="41"/>
-      <c r="D104" s="41"/>
-      <c r="E104" s="41"/>
+      <c r="C104" s="52"/>
+      <c r="D104" s="52"/>
+      <c r="E104" s="52"/>
       <c r="F104" s="9"/>
     </row>
     <row r="105" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5868,7 +7549,7 @@
       <c r="E105" s="14">
         <v>247792</v>
       </c>
-      <c r="F105" s="46" t="s">
+      <c r="F105" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5885,7 +7566,7 @@
       <c r="E106" s="14">
         <v>785826</v>
       </c>
-      <c r="F106" s="46" t="s">
+      <c r="F106" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5896,13 +7577,13 @@
       <c r="C107" s="4">
         <v>4123</v>
       </c>
-      <c r="D107" s="49" t="s">
+      <c r="D107" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E107" s="49" t="s">
+      <c r="E107" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F107" s="46" t="s">
+      <c r="F107" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5919,7 +7600,7 @@
       <c r="E108" s="14">
         <v>12385</v>
       </c>
-      <c r="F108" s="46" t="s">
+      <c r="F108" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5936,7 +7617,7 @@
       <c r="E109" s="14">
         <v>40310</v>
       </c>
-      <c r="F109" s="46" t="s">
+      <c r="F109" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5947,23 +7628,23 @@
       <c r="C110" s="12">
         <v>4100</v>
       </c>
-      <c r="D110" s="46">
+      <c r="D110" s="33">
         <v>168071</v>
       </c>
-      <c r="E110" s="46">
+      <c r="E110" s="33">
         <v>186299</v>
       </c>
-      <c r="F110" s="46" t="s">
+      <c r="F110" s="33" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="111" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="38" t="s">
+      <c r="B111" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="C111" s="39"/>
-      <c r="D111" s="39"/>
-      <c r="E111" s="39"/>
+      <c r="C111" s="56"/>
+      <c r="D111" s="56"/>
+      <c r="E111" s="56"/>
       <c r="F111" s="9"/>
     </row>
     <row r="112" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5973,23 +7654,23 @@
       <c r="C112" s="12">
         <v>4210</v>
       </c>
-      <c r="D112" s="46">
+      <c r="D112" s="33">
         <v>1788073</v>
       </c>
-      <c r="E112" s="46">
+      <c r="E112" s="33">
         <v>3004731</v>
       </c>
-      <c r="F112" s="46" t="s">
+      <c r="F112" s="33" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="113" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="40" t="s">
+      <c r="B113" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="C113" s="41"/>
-      <c r="D113" s="41"/>
-      <c r="E113" s="41"/>
+      <c r="C113" s="52"/>
+      <c r="D113" s="52"/>
+      <c r="E113" s="52"/>
       <c r="F113" s="9"/>
     </row>
     <row r="114" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -5999,13 +7680,13 @@
       <c r="C114" s="4">
         <v>4211</v>
       </c>
-      <c r="D114" s="49">
+      <c r="D114" s="34">
         <v>19625</v>
       </c>
-      <c r="E114" s="49">
+      <c r="E114" s="34">
         <v>8130</v>
       </c>
-      <c r="F114" s="46" t="s">
+      <c r="F114" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6016,13 +7697,13 @@
       <c r="C115" s="4">
         <v>4212</v>
       </c>
-      <c r="D115" s="49" t="s">
+      <c r="D115" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="49" t="s">
+      <c r="E115" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F115" s="46" t="s">
+      <c r="F115" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6033,13 +7714,13 @@
       <c r="C116" s="4">
         <v>4213</v>
       </c>
-      <c r="D116" s="49">
+      <c r="D116" s="34">
         <v>1757000</v>
       </c>
-      <c r="E116" s="49">
+      <c r="E116" s="34">
         <v>2990000</v>
       </c>
-      <c r="F116" s="46" t="s">
+      <c r="F116" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6050,13 +7731,13 @@
       <c r="C117" s="4">
         <v>4214</v>
       </c>
-      <c r="D117" s="49">
+      <c r="D117" s="34">
         <v>11448</v>
       </c>
-      <c r="E117" s="49">
+      <c r="E117" s="34">
         <v>6601</v>
       </c>
-      <c r="F117" s="46" t="s">
+      <c r="F117" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6067,13 +7748,13 @@
       <c r="C118" s="4">
         <v>4219</v>
       </c>
-      <c r="D118" s="49" t="s">
+      <c r="D118" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E118" s="49" t="s">
+      <c r="E118" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F118" s="46" t="s">
+      <c r="F118" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6084,23 +7765,23 @@
       <c r="C119" s="12">
         <v>4220</v>
       </c>
-      <c r="D119" s="50">
+      <c r="D119" s="35">
         <v>1955542</v>
       </c>
-      <c r="E119" s="50">
+      <c r="E119" s="35">
         <v>3248793</v>
       </c>
-      <c r="F119" s="46" t="s">
+      <c r="F119" s="33" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="120" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="40" t="s">
+      <c r="B120" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="C120" s="41"/>
-      <c r="D120" s="41"/>
-      <c r="E120" s="41"/>
+      <c r="C120" s="52"/>
+      <c r="D120" s="52"/>
+      <c r="E120" s="52"/>
       <c r="F120" s="9"/>
     </row>
     <row r="121" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6116,21 +7797,21 @@
       <c r="E121" s="14">
         <v>131793</v>
       </c>
-      <c r="F121" s="46" t="s">
+      <c r="F121" s="33" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B122" s="42" t="s">
+      <c r="B122" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="C122" s="42">
+      <c r="C122" s="53">
         <v>4222</v>
       </c>
-      <c r="D122" s="51" t="s">
+      <c r="D122" s="57" t="s">
         <v>154</v>
       </c>
-      <c r="E122" s="51" t="s">
+      <c r="E122" s="57" t="s">
         <v>154</v>
       </c>
       <c r="F122" s="47" t="s">
@@ -6138,10 +7819,10 @@
       </c>
     </row>
     <row r="123" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="43"/>
-      <c r="C123" s="43"/>
-      <c r="D123" s="52"/>
-      <c r="E123" s="52"/>
+      <c r="B123" s="54"/>
+      <c r="C123" s="54"/>
+      <c r="D123" s="58"/>
+      <c r="E123" s="58"/>
       <c r="F123" s="48"/>
     </row>
     <row r="124" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6157,7 +7838,7 @@
       <c r="E124" s="14">
         <v>3117000</v>
       </c>
-      <c r="F124" s="46" t="s">
+      <c r="F124" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6168,13 +7849,13 @@
       <c r="C125" s="4">
         <v>4224</v>
       </c>
-      <c r="D125" s="49" t="s">
+      <c r="D125" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E125" s="49" t="s">
+      <c r="E125" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F125" s="46" t="s">
+      <c r="F125" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6185,13 +7866,13 @@
       <c r="C126" s="4">
         <v>4229</v>
       </c>
-      <c r="D126" s="49" t="s">
+      <c r="D126" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="49" t="s">
+      <c r="E126" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F126" s="46" t="s">
+      <c r="F126" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6202,13 +7883,13 @@
       <c r="C127" s="12">
         <v>4200</v>
       </c>
-      <c r="D127" s="50">
-        <v>167469</v>
-      </c>
-      <c r="E127" s="50">
-        <v>244062</v>
-      </c>
-      <c r="F127" s="46" t="s">
+      <c r="D127" s="35">
+        <v>-167469</v>
+      </c>
+      <c r="E127" s="35">
+        <v>-244062</v>
+      </c>
+      <c r="F127" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6230,12 +7911,12 @@
       </c>
     </row>
     <row r="129" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="44" t="s">
+      <c r="B129" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="C129" s="45"/>
-      <c r="D129" s="45"/>
-      <c r="E129" s="36" t="s">
+      <c r="C129" s="50"/>
+      <c r="D129" s="50"/>
+      <c r="E129" s="31" t="s">
         <v>3</v>
       </c>
       <c r="F129" s="9"/>
@@ -6247,23 +7928,23 @@
       <c r="C130" s="12">
         <v>4310</v>
       </c>
-      <c r="D130" s="46" t="s">
+      <c r="D130" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E130" s="46">
+      <c r="E130" s="33">
         <v>59100</v>
       </c>
-      <c r="F130" s="46" t="s">
+      <c r="F130" s="33" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="131" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="40" t="s">
+      <c r="B131" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="C131" s="41"/>
-      <c r="D131" s="41"/>
-      <c r="E131" s="37"/>
+      <c r="C131" s="52"/>
+      <c r="D131" s="52"/>
+      <c r="E131" s="32"/>
       <c r="F131" s="9"/>
     </row>
     <row r="132" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6273,13 +7954,13 @@
       <c r="C132" s="4">
         <v>4311</v>
       </c>
-      <c r="D132" s="49" t="s">
+      <c r="D132" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="49" t="s">
+      <c r="E132" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F132" s="46" t="s">
+      <c r="F132" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6290,13 +7971,13 @@
       <c r="C133" s="4">
         <v>4312</v>
       </c>
-      <c r="D133" s="49" t="s">
+      <c r="D133" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="49" t="s">
+      <c r="E133" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F133" s="46" t="s">
+      <c r="F133" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6307,13 +7988,13 @@
       <c r="C134" s="4">
         <v>4313</v>
       </c>
-      <c r="D134" s="49" t="s">
+      <c r="D134" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E134" s="49">
+      <c r="E134" s="34">
         <v>59100</v>
       </c>
-      <c r="F134" s="46" t="s">
+      <c r="F134" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6324,13 +8005,13 @@
       <c r="C135" s="4">
         <v>4314</v>
       </c>
-      <c r="D135" s="49" t="s">
+      <c r="D135" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E135" s="49" t="s">
+      <c r="E135" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F135" s="46" t="s">
+      <c r="F135" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6341,13 +8022,13 @@
       <c r="C136" s="4">
         <v>4319</v>
       </c>
-      <c r="D136" s="49" t="s">
+      <c r="D136" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E136" s="49" t="s">
+      <c r="E136" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F136" s="46" t="s">
+      <c r="F136" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6358,23 +8039,23 @@
       <c r="C137" s="12">
         <v>4320</v>
       </c>
-      <c r="D137" s="46" t="s">
+      <c r="D137" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E137" s="50">
+      <c r="E137" s="35">
         <v>498</v>
       </c>
-      <c r="F137" s="46" t="s">
+      <c r="F137" s="33" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="138" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="40" t="s">
+      <c r="B138" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="C138" s="41"/>
-      <c r="D138" s="41"/>
-      <c r="E138" s="37"/>
+      <c r="C138" s="52"/>
+      <c r="D138" s="52"/>
+      <c r="E138" s="32"/>
       <c r="F138" s="9"/>
     </row>
     <row r="139" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6384,13 +8065,13 @@
       <c r="C139" s="4">
         <v>4321</v>
       </c>
-      <c r="D139" s="49" t="s">
+      <c r="D139" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E139" s="49" t="s">
+      <c r="E139" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F139" s="46" t="s">
+      <c r="F139" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6401,13 +8082,13 @@
       <c r="C140" s="4">
         <v>4322</v>
       </c>
-      <c r="D140" s="49" t="s">
+      <c r="D140" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E140" s="49" t="s">
+      <c r="E140" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F140" s="46" t="s">
+      <c r="F140" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6418,13 +8099,13 @@
       <c r="C141" s="4">
         <v>4323</v>
       </c>
-      <c r="D141" s="49" t="s">
+      <c r="D141" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E141" s="49" t="s">
+      <c r="E141" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F141" s="46" t="s">
+      <c r="F141" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6435,13 +8116,13 @@
       <c r="C142" s="4">
         <v>4329</v>
       </c>
-      <c r="D142" s="53" t="s">
+      <c r="D142" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E142" s="54">
+      <c r="E142" s="37">
         <v>498</v>
       </c>
-      <c r="F142" s="46" t="s">
+      <c r="F142" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6452,13 +8133,13 @@
       <c r="C143" s="12">
         <v>4300</v>
       </c>
-      <c r="D143" s="55" t="s">
+      <c r="D143" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="E143" s="55">
+      <c r="E143" s="38">
         <v>58602</v>
       </c>
-      <c r="F143" s="46" t="s">
+      <c r="F143" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6469,19 +8150,19 @@
       <c r="C144" s="12">
         <v>4400</v>
       </c>
-      <c r="D144" s="55">
+      <c r="D144" s="38">
         <v>602</v>
       </c>
-      <c r="E144" s="55">
+      <c r="E144" s="38">
         <v>839</v>
       </c>
-      <c r="F144" s="46" t="s">
+      <c r="F144" s="33" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="145" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="146" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="56" t="s">
+      <c r="B146" s="39" t="s">
         <v>155</v>
       </c>
       <c r="C146" s="21" t="s">
@@ -6498,58 +8179,58 @@
       </c>
     </row>
     <row r="147" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="31" t="s">
+      <c r="B147" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="C147" s="59">
+      <c r="C147" s="42">
         <v>2110</v>
       </c>
-      <c r="D147" s="60">
+      <c r="D147" s="43">
         <v>1480393</v>
       </c>
-      <c r="E147" s="60">
+      <c r="E147" s="43">
         <v>1239683</v>
       </c>
-      <c r="F147" s="60" t="s">
+      <c r="F147" s="43" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="148" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="31" t="s">
+      <c r="B148" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="C148" s="59">
+      <c r="C148" s="42">
         <v>2120</v>
       </c>
-      <c r="D148" s="50">
+      <c r="D148" s="35">
         <v>1245765</v>
       </c>
-      <c r="E148" s="50">
+      <c r="E148" s="35">
         <v>1008066</v>
       </c>
-      <c r="F148" s="58" t="s">
+      <c r="F148" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="149" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="57" t="s">
+      <c r="B149" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="C149" s="59">
+      <c r="C149" s="42">
         <v>2100</v>
       </c>
-      <c r="D149" s="60">
+      <c r="D149" s="43">
         <v>234628</v>
       </c>
-      <c r="E149" s="60">
+      <c r="E149" s="43">
         <v>231617</v>
       </c>
-      <c r="F149" s="58" t="s">
+      <c r="F149" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="150" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="31" t="s">
+      <c r="B150" s="27" t="s">
         <v>160</v>
       </c>
       <c r="C150" s="25">
@@ -6561,12 +8242,12 @@
       <c r="E150" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="F150" s="58" t="s">
+      <c r="F150" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="151" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="31" t="s">
+      <c r="B151" s="27" t="s">
         <v>161</v>
       </c>
       <c r="C151" s="25">
@@ -6578,63 +8259,63 @@
       <c r="E151" s="14">
         <v>128457</v>
       </c>
-      <c r="F151" s="58" t="s">
+      <c r="F151" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="152" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="57" t="s">
+      <c r="B152" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="C152" s="59">
+      <c r="C152" s="42">
         <v>2200</v>
       </c>
-      <c r="D152" s="60">
+      <c r="D152" s="43">
         <v>81183</v>
       </c>
-      <c r="E152" s="60">
+      <c r="E152" s="43">
         <v>103160</v>
       </c>
-      <c r="F152" s="58" t="s">
+      <c r="F152" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="153" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="31" t="s">
+      <c r="B153" s="27" t="s">
         <v>163</v>
       </c>
       <c r="C153" s="25">
         <v>2310</v>
       </c>
-      <c r="D153" s="58" t="s">
+      <c r="D153" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E153" s="58" t="s">
+      <c r="E153" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="F153" s="58" t="s">
+      <c r="F153" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="154" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="31" t="s">
+      <c r="B154" s="27" t="s">
         <v>164</v>
       </c>
       <c r="C154" s="25">
         <v>2320</v>
       </c>
-      <c r="D154" s="58">
+      <c r="D154" s="41">
         <v>11853</v>
       </c>
-      <c r="E154" s="58">
+      <c r="E154" s="41">
         <v>8086</v>
       </c>
-      <c r="F154" s="58" t="s">
+      <c r="F154" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="155" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="31" t="s">
+      <c r="B155" s="27" t="s">
         <v>165</v>
       </c>
       <c r="C155" s="25">
@@ -6646,131 +8327,131 @@
       <c r="E155" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="F155" s="58" t="s">
+      <c r="F155" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="156" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="31" t="s">
+      <c r="B156" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="C156" s="59">
+      <c r="C156" s="42">
         <v>2340</v>
       </c>
-      <c r="D156" s="60">
+      <c r="D156" s="43">
         <v>26848</v>
       </c>
-      <c r="E156" s="60">
+      <c r="E156" s="43">
         <v>35160</v>
       </c>
-      <c r="F156" s="58" t="s">
+      <c r="F156" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="157" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="31" t="s">
+      <c r="B157" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="C157" s="59">
+      <c r="C157" s="42">
         <v>2350</v>
       </c>
-      <c r="D157" s="50">
+      <c r="D157" s="35">
         <v>57107</v>
       </c>
-      <c r="E157" s="50">
+      <c r="E157" s="35">
         <v>52741</v>
       </c>
-      <c r="F157" s="58" t="s">
+      <c r="F157" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="158" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="57" t="s">
+      <c r="B158" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="C158" s="59">
+      <c r="C158" s="42">
         <v>2300</v>
       </c>
-      <c r="D158" s="60">
+      <c r="D158" s="43">
         <v>62777</v>
       </c>
-      <c r="E158" s="60">
+      <c r="E158" s="43">
         <v>93665</v>
       </c>
-      <c r="F158" s="58" t="s">
+      <c r="F158" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="159" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="31" t="s">
+      <c r="B159" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="C159" s="59">
+      <c r="C159" s="42">
         <v>2410</v>
       </c>
-      <c r="D159" s="50">
+      <c r="D159" s="35">
         <v>15457</v>
       </c>
-      <c r="E159" s="50">
+      <c r="E159" s="35">
         <v>24487</v>
       </c>
-      <c r="F159" s="58" t="s">
+      <c r="F159" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="160" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="31" t="s">
+      <c r="B160" s="27" t="s">
         <v>170</v>
       </c>
       <c r="C160" s="25">
         <v>2421</v>
       </c>
-      <c r="D160" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="E160" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="F160" s="58" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="161" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="31" t="s">
+      <c r="D160" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E160" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F160" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B161" s="27" t="s">
         <v>171</v>
       </c>
       <c r="C161" s="25">
         <v>2430</v>
       </c>
-      <c r="D161" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="E161" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="F161" s="58" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="162" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="31" t="s">
+      <c r="D161" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E161" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F161" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B162" s="27" t="s">
         <v>172</v>
       </c>
       <c r="C162" s="25">
         <v>2450</v>
       </c>
-      <c r="D162" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="E162" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="F162" s="58" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="163" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="31" t="s">
+      <c r="D162" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E162" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F162" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B163" s="27" t="s">
         <v>173</v>
       </c>
       <c r="C163" s="25">
@@ -6779,32 +8460,32 @@
       <c r="D163" s="14">
         <v>184</v>
       </c>
-      <c r="E163" s="58">
+      <c r="E163" s="41">
         <v>1962</v>
       </c>
-      <c r="F163" s="58" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="164" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="57" t="s">
+      <c r="F163" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B164" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="C164" s="59">
+      <c r="C164" s="42">
         <v>2400</v>
       </c>
-      <c r="D164" s="60">
+      <c r="D164" s="43">
         <v>47417</v>
       </c>
-      <c r="E164" s="60">
+      <c r="E164" s="43">
         <v>72431</v>
       </c>
-      <c r="F164" s="58" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="165" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="166" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F164" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="166" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H166" s="20" t="s">
         <v>78</v>
       </c>
@@ -6824,7 +8505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H167" s="23" t="s">
         <v>175</v>
       </c>
@@ -6834,17 +8515,24 @@
       <c r="J167" s="25">
         <v>2110</v>
       </c>
-      <c r="K167" s="58">
+      <c r="K167" s="41">
         <v>1480393</v>
       </c>
-      <c r="L167" s="58">
+      <c r="L167" s="41">
         <v>1239683</v>
       </c>
       <c r="M167" s="25" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="168" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O167" t="s">
+        <v>220</v>
+      </c>
+      <c r="P167" s="15">
+        <f>K167-K168-K170-K171</f>
+        <v>81183</v>
+      </c>
+    </row>
+    <row r="168" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H168" s="23" t="s">
         <v>177</v>
       </c>
@@ -6864,8 +8552,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H169" s="34" t="s">
+    <row r="169" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H169" s="29" t="s">
         <v>179</v>
       </c>
       <c r="I169" s="24" t="s">
@@ -6874,17 +8562,17 @@
       <c r="J169" s="25">
         <v>2100</v>
       </c>
-      <c r="K169" s="58">
+      <c r="K169" s="41">
         <v>234628</v>
       </c>
-      <c r="L169" s="58">
+      <c r="L169" s="41">
         <v>231617</v>
       </c>
       <c r="M169" s="25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H170" s="23" t="s">
         <v>181</v>
       </c>
@@ -6904,7 +8592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H171" s="23" t="s">
         <v>182</v>
       </c>
@@ -6924,8 +8612,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H172" s="31" t="s">
+    <row r="172" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H172" s="27" t="s">
         <v>183</v>
       </c>
       <c r="I172" s="24" t="s">
@@ -6934,18 +8622,18 @@
       <c r="J172" s="25">
         <v>2200</v>
       </c>
-      <c r="K172" s="58">
+      <c r="K172" s="41">
         <v>81183</v>
       </c>
-      <c r="L172" s="58">
+      <c r="L172" s="41">
         <v>103160</v>
       </c>
       <c r="M172" s="25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H173" s="31" t="s">
+    <row r="173" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H173" s="27" t="s">
         <v>185</v>
       </c>
       <c r="I173" s="24" t="s">
@@ -6964,8 +8652,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H174" s="31" t="s">
+    <row r="174" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H174" s="27" t="s">
         <v>187</v>
       </c>
       <c r="I174" s="24" t="s">
@@ -6974,18 +8662,18 @@
       <c r="J174" s="25">
         <v>2340</v>
       </c>
-      <c r="K174" s="58">
+      <c r="K174" s="41">
         <v>26848</v>
       </c>
-      <c r="L174" s="58">
+      <c r="L174" s="41">
         <v>35160</v>
       </c>
       <c r="M174" s="25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H175" s="31" t="s">
+    <row r="175" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H175" s="27" t="s">
         <v>188</v>
       </c>
       <c r="I175" s="24" t="s">
@@ -7004,8 +8692,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H176" s="31" t="s">
+    <row r="176" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H176" s="27" t="s">
         <v>189</v>
       </c>
       <c r="I176" s="24" t="s">
@@ -7014,10 +8702,10 @@
       <c r="J176" s="25">
         <v>2300</v>
       </c>
-      <c r="K176" s="58">
+      <c r="K176" s="41">
         <v>62777</v>
       </c>
-      <c r="L176" s="58">
+      <c r="L176" s="41">
         <v>93665</v>
       </c>
       <c r="M176" s="25" t="s">
@@ -7066,7 +8754,7 @@
       </c>
     </row>
     <row r="180" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H180" s="31" t="s">
+      <c r="H180" s="27" t="s">
         <v>194</v>
       </c>
       <c r="I180" s="24" t="s">
@@ -7075,10 +8763,10 @@
       <c r="J180" s="25">
         <v>2400</v>
       </c>
-      <c r="K180" s="58">
+      <c r="K180" s="41">
         <v>47417</v>
       </c>
-      <c r="L180" s="58">
+      <c r="L180" s="41">
         <v>47417</v>
       </c>
       <c r="M180" s="25" t="s">
@@ -7086,7 +8774,7 @@
       </c>
     </row>
     <row r="181" spans="8:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H181" s="34" t="s">
+      <c r="H181" s="29" t="s">
         <v>196</v>
       </c>
       <c r="I181" s="24" t="s">
@@ -7095,11 +8783,11 @@
       <c r="J181" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="K181" s="63">
+      <c r="K181" s="46">
         <f>K169/K167</f>
         <v>0.15849034682006738</v>
       </c>
-      <c r="L181" s="63">
+      <c r="L181" s="46">
         <f>L169/L167</f>
         <v>0.18683566685999567</v>
       </c>
@@ -7108,20 +8796,20 @@
       </c>
     </row>
     <row r="182" spans="8:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H182" s="34" t="s">
+      <c r="H182" s="29" t="s">
         <v>198</v>
       </c>
       <c r="I182" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="J182" s="61" t="s">
+      <c r="J182" s="44" t="s">
         <v>216</v>
       </c>
-      <c r="K182" s="63">
+      <c r="K182" s="46">
         <f>K172/K167</f>
         <v>5.4838816449415795E-2</v>
       </c>
-      <c r="L182" s="63">
+      <c r="L182" s="46">
         <f>L172/L167</f>
         <v>8.3214821853651297E-2</v>
       </c>
@@ -7139,11 +8827,11 @@
       <c r="J183" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="K183" s="63">
+      <c r="K183" s="46">
         <f>K168/K167</f>
         <v>0.84150965317993265</v>
       </c>
-      <c r="L183" s="63">
+      <c r="L183" s="46">
         <f>L168/L167</f>
         <v>0.81316433314000436</v>
       </c>
@@ -7161,11 +8849,11 @@
       <c r="J184" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="K184" s="63">
+      <c r="K184" s="46">
         <f>K170/K167</f>
         <v>0</v>
       </c>
-      <c r="L184" s="63">
+      <c r="L184" s="46">
         <f>L170/L167</f>
         <v>0</v>
       </c>
@@ -7183,11 +8871,11 @@
       <c r="J185" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="K185" s="63">
+      <c r="K185" s="46">
         <f>K171/K167</f>
         <v>0.10365153037065157</v>
       </c>
-      <c r="L185" s="63">
+      <c r="L185" s="46">
         <f>L171/L167</f>
         <v>0.10362084500634436</v>
       </c>
@@ -7205,11 +8893,11 @@
       <c r="J186" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="K186" s="63">
+      <c r="K186" s="46">
         <f>K173/K167</f>
         <v>0</v>
       </c>
-      <c r="L186" s="63">
+      <c r="L186" s="46">
         <f>L173/L167</f>
         <v>0</v>
       </c>
@@ -7227,11 +8915,11 @@
       <c r="J187" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="K187" s="63">
+      <c r="K187" s="46">
         <f>K176/K167</f>
         <v>4.2405631477587372E-2</v>
       </c>
-      <c r="L187" s="63">
+      <c r="L187" s="46">
         <f>L176/L167</f>
         <v>7.5555605747598384E-2</v>
       </c>
@@ -7249,11 +8937,11 @@
       <c r="J188" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="K188" s="63">
+      <c r="K188" s="46">
         <f>K175/K167</f>
         <v>3.8575567433782786E-2</v>
       </c>
-      <c r="L188" s="63">
+      <c r="L188" s="46">
         <f>L175/L167</f>
         <v>4.2543940668703206E-2</v>
       </c>
@@ -7262,29 +8950,29 @@
       </c>
     </row>
     <row r="189" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="I189" s="62"/>
+      <c r="I189" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="H78:H79"/>
+    <mergeCell ref="I78:I79"/>
+    <mergeCell ref="K78:K79"/>
+    <mergeCell ref="L78:L79"/>
+    <mergeCell ref="M78:M79"/>
+    <mergeCell ref="B98:E98"/>
+    <mergeCell ref="B104:E104"/>
+    <mergeCell ref="B111:E111"/>
+    <mergeCell ref="B113:E113"/>
+    <mergeCell ref="B120:E120"/>
     <mergeCell ref="F122:F123"/>
     <mergeCell ref="B129:D129"/>
     <mergeCell ref="B131:D131"/>
     <mergeCell ref="B138:D138"/>
     <mergeCell ref="B122:B123"/>
-    <mergeCell ref="B98:E98"/>
-    <mergeCell ref="B104:E104"/>
-    <mergeCell ref="B111:E111"/>
-    <mergeCell ref="B113:E113"/>
-    <mergeCell ref="B120:E120"/>
     <mergeCell ref="C122:C123"/>
     <mergeCell ref="D122:D123"/>
     <mergeCell ref="E122:E123"/>
-    <mergeCell ref="H78:H79"/>
-    <mergeCell ref="I78:I79"/>
-    <mergeCell ref="K78:K79"/>
-    <mergeCell ref="L78:L79"/>
-    <mergeCell ref="M78:M79"/>
-    <mergeCell ref="B96:E96"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>